<commit_message>
New file structure and test files modified
</commit_message>
<xml_diff>
--- a/Tests/Files/test2.xlsx
+++ b/Tests/Files/test2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wiktorgrochowski/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wiktorgrochowski/Desktop/editorCSV/Tests/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E4A6B1-7A6C-0D4F-85C0-EAB0653DE36B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF0AE8D-47D4-E247-97BE-97CB6E2E4A89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{FD608FCB-094B-184A-A633-0E8BBBE66A3E}"/>
   </bookViews>
@@ -49,10 +49,10 @@
     <t>Grochowsk</t>
   </si>
   <si>
-    <t>Micheal</t>
-  </si>
-  <si>
     <t>Groch</t>
+  </si>
+  <si>
+    <t>wiktor</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,10 +506,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -517,10 +517,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>26</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>27</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>28</v>
@@ -550,10 +550,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>29</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>31</v>

</xml_diff>